<commit_message>
Draw bar chart of good intervals
This may not be what we won't, just a try.
</commit_message>
<xml_diff>
--- a/good_intervals.xlsx
+++ b/good_intervals.xlsx
@@ -124,6 +124,147 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Bar Chart</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Sheet'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$A$2:$A$34</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$B$2:$B$34</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+          <max val="1"/>
+          <min val="0"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Concentration</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -408,81 +549,366 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>init time=1639275694</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>end</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>grade</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1639189492</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0:00</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>1639189552</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.86</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1639189558</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1:03</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>1639189618</v>
-      </c>
-      <c r="C3" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2:16</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3:21</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4:28</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5:43</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6:44</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7:50</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>8:52</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>9:54</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12:24</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13:28</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14:31</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16:37</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18:39</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>22:44</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>23:47</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>24:55</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>25:56</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>26:58</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>28:05</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>29:11</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>30:12</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>31:14</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>33:12</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>34:57</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
         <v>0.66</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1639189624</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1639189684</v>
-      </c>
-      <c r="C4" t="n">
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>36:05</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>37:07</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
         <v>0.6899999999999999</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1639189687</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1639189747</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>